<commit_message>
Add description in README file
</commit_message>
<xml_diff>
--- a/doc/table.xlsx
+++ b/doc/table.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20381"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\projs\php\park\park\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8597D5C5-AD17-4704-A48F-2E41A78943FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19335" windowHeight="9345" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19335" windowHeight="9345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="用户" sheetId="1" r:id="rId1"/>
@@ -24,7 +30,6 @@
     <sheet name="群发私信" sheetId="15" r:id="rId15"/>
     <sheet name="入出金" sheetId="16" r:id="rId16"/>
     <sheet name="x存款" sheetId="17" r:id="rId17"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -689,8 +694,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,11 +816,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -857,7 +870,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,9 +902,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,6 +954,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1098,21 +1147,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="65.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1169,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1186,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -1145,7 +1194,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -1156,7 +1205,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -1167,7 +1216,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -1178,7 +1227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -1189,7 +1238,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -1200,7 +1249,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>115</v>
       </c>
@@ -1211,7 +1260,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1271,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1230,7 +1279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -1238,7 +1287,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1246,7 +1295,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1261,21 +1310,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +1332,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1300,7 +1349,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1308,7 +1357,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1319,7 +1368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -1330,7 +1379,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -1341,7 +1390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1352,7 +1401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1363,7 +1412,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -1374,7 +1423,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>160</v>
       </c>
@@ -1393,21 +1442,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1464,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1432,7 +1481,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1440,7 +1489,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -1451,7 +1500,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1462,7 +1511,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1473,7 +1522,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1484,7 +1533,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1495,7 +1544,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1506,7 +1555,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1517,7 +1566,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1528,7 +1577,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="5" t="s">
         <v>149</v>
       </c>
@@ -1540,21 +1589,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +1628,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1587,7 +1636,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1598,7 +1647,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1609,7 +1658,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -1620,7 +1669,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1631,7 +1680,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -1642,7 +1691,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -1653,7 +1702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1664,7 +1713,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1675,7 +1724,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1693,21 +1742,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="92.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1718,7 +1767,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1735,7 +1784,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1743,7 +1792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -1751,7 +1800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1759,7 +1808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1767,7 +1816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1775,7 +1824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1783,22 +1832,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C14" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C15" s="5" t="s">
         <v>149</v>
       </c>
@@ -1810,21 +1859,21 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="92.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1832,7 +1881,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1849,7 +1898,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1857,7 +1906,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -1868,7 +1917,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1879,7 +1928,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -1890,7 +1939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1898,7 +1947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1906,7 +1955,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -1914,7 +1963,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1922,7 +1971,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1940,21 +1989,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A2:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="92.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +2011,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1979,7 +2028,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1987,7 +2036,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1995,7 +2044,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2010,21 +2059,21 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="92.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2049,7 +2098,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2057,7 +2106,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2068,7 +2117,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2079,7 +2128,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2090,7 +2139,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2098,7 +2147,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2106,7 +2155,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -2114,7 +2163,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -2129,21 +2178,21 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="92.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2154,7 +2203,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2171,7 +2220,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -2179,7 +2228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -2193,37 +2242,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.75" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="65.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2265,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2248,7 +2282,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -2256,7 +2290,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -2267,7 +2301,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -2278,7 +2312,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2289,7 +2323,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -2297,7 +2331,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -2305,7 +2339,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2313,7 +2347,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2328,7 +2362,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
@@ -2338,14 +2372,14 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2387,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2404,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2378,7 +2412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2394,24 +2428,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
   <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2436,7 +2470,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2444,7 +2478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2459,7 +2493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
@@ -2469,14 +2503,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2501,7 +2535,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2509,7 +2543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2517,7 +2551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2532,7 +2566,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
@@ -2542,14 +2576,14 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2591,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2574,7 +2608,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -2582,7 +2616,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +2624,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2598,12 +2632,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2615,21 +2649,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2654,7 +2688,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2662,7 +2696,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2670,7 +2704,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2681,7 +2715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2692,7 +2726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2703,7 +2737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2714,7 +2748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2732,7 +2766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="1" tint="0.34998626667073579"/>
   </sheetPr>
@@ -2742,14 +2776,14 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="25.375" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2757,7 +2791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2774,7 +2808,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2782,12 +2816,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2795,7 +2829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2803,7 +2837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2811,7 +2845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2819,7 +2853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2834,21 +2868,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2856,7 +2890,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2873,7 +2907,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2881,7 +2915,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -2892,7 +2926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -2903,7 +2937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2914,7 +2948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -2925,7 +2959,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2936,7 +2970,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2947,7 +2981,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C13" s="5" t="s">
         <v>152</v>
       </c>

</xml_diff>